<commit_message>
Created first draft of UseCase Diagramm
</commit_message>
<xml_diff>
--- a/Timetable/Reichmann.xlsx
+++ b/Timetable/Reichmann.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="525" windowWidth="20115" windowHeight="8085"/>
   </bookViews>
   <sheets>
-    <sheet name="Fegerl Michael" sheetId="1" r:id="rId1"/>
+    <sheet name="Daniel Reichmann" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>date</t>
   </si>
@@ -33,12 +33,18 @@
   <si>
     <t>comment</t>
   </si>
+  <si>
+    <t>UseCase</t>
+  </si>
+  <si>
+    <t>Draft, needs aprovement</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,7 +292,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -360,6 +366,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -394,6 +401,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -569,14 +577,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -586,7 +594,7 @@
     <col min="6" max="6" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -607,19 +615,29 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>41666</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="D2" s="11">
         <f t="shared" ref="D2:D66" si="0">C2-B2</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="7"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -630,7 +648,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -642,7 +660,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -654,7 +672,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -666,7 +684,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -678,7 +696,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -690,7 +708,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -702,7 +720,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -714,7 +732,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -726,7 +744,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -738,7 +756,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -750,7 +768,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -762,7 +780,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -774,7 +792,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -786,7 +804,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -798,7 +816,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -810,7 +828,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1">
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -822,7 +840,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -834,7 +852,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -846,7 +864,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1">
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -858,7 +876,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1">
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -870,7 +888,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1">
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -882,7 +900,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1">
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -894,7 +912,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1">
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -906,7 +924,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1">
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -918,7 +936,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -930,7 +948,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1">
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -942,7 +960,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1">
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -954,7 +972,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1">
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -966,7 +984,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1">
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -978,7 +996,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1">
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -990,7 +1008,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1">
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1002,7 +1020,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1">
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1014,7 +1032,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1">
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1026,7 +1044,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1">
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1038,7 +1056,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1">
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1050,7 +1068,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1">
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1062,7 +1080,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1">
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1074,7 +1092,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1">
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1086,7 +1104,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1">
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1098,7 +1116,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1">
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1110,7 +1128,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1">
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1122,7 +1140,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1">
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1134,7 +1152,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1">
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1146,7 +1164,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1">
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1158,7 +1176,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1">
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1170,7 +1188,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="1:7" ht="15.75" thickBot="1">
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1182,7 +1200,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" ht="15.75" thickBot="1">
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1194,7 +1212,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="1:7" ht="15.75" thickBot="1">
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1206,7 +1224,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="2"/>
     </row>
-    <row r="52" spans="1:7" ht="15.75" thickBot="1">
+    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1218,7 +1236,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="1:7" ht="15.75" thickBot="1">
+    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1230,7 +1248,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="1:7" ht="15.75" thickBot="1">
+    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1242,7 +1260,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="1:7" ht="15.75" thickBot="1">
+    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1254,7 +1272,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:7" ht="15.75" thickBot="1">
+    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1266,7 +1284,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="2"/>
     </row>
-    <row r="57" spans="1:7" ht="15.75" thickBot="1">
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1278,7 +1296,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="1:7" ht="15.75" thickBot="1">
+    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1290,7 +1308,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:7" ht="15.75" thickBot="1">
+    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1302,7 +1320,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="1:7" ht="15.75" thickBot="1">
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1314,7 +1332,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:7" ht="15.75" thickBot="1">
+    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1326,7 +1344,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="1:7" ht="15.75" thickBot="1">
+    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1338,7 +1356,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" spans="1:7" ht="15.75" thickBot="1">
+    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1350,7 +1368,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="2"/>
     </row>
-    <row r="64" spans="1:7" ht="15.75" thickBot="1">
+    <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1362,7 +1380,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="2"/>
     </row>
-    <row r="65" spans="1:7" ht="15.75" thickBot="1">
+    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1374,7 +1392,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="2"/>
     </row>
-    <row r="66" spans="1:7" ht="15.75" thickBot="1">
+    <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1386,7 +1404,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="2"/>
     </row>
-    <row r="67" spans="1:7" ht="15.75" thickBot="1">
+    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1398,7 +1416,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="1:7" ht="15.75" thickBot="1">
+    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1410,7 +1428,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="2"/>
     </row>
-    <row r="69" spans="1:7" ht="15.75" thickBot="1">
+    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1422,7 +1440,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="2"/>
     </row>
-    <row r="70" spans="1:7" ht="15.75" thickBot="1">
+    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1434,7 +1452,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="2"/>
     </row>
-    <row r="71" spans="1:7" ht="15.75" thickBot="1">
+    <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1446,7 +1464,7 @@
       <c r="F71" s="7"/>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="1:7" ht="15.75" thickBot="1">
+    <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1458,7 +1476,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="2"/>
     </row>
-    <row r="73" spans="1:7" ht="15.75" thickBot="1">
+    <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1470,7 +1488,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="1:7" ht="15.75" thickBot="1">
+    <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1482,7 +1500,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="1:7" ht="15.75" thickBot="1">
+    <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1494,7 +1512,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="1:7" ht="15.75" thickBot="1">
+    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1506,7 +1524,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="1:7" ht="15.75" thickBot="1">
+    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1518,7 +1536,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="2"/>
     </row>
-    <row r="78" spans="1:7" ht="15.75" thickBot="1">
+    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="6"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1530,7 +1548,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="2"/>
     </row>
-    <row r="79" spans="1:7" ht="15.75" thickBot="1">
+    <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1542,7 +1560,7 @@
       <c r="F79" s="7"/>
       <c r="G79" s="2"/>
     </row>
-    <row r="80" spans="1:7" ht="15.75" thickBot="1">
+    <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1554,7 +1572,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="2"/>
     </row>
-    <row r="81" spans="1:7" ht="15.75" thickBot="1">
+    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1566,7 +1584,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="2"/>
     </row>
-    <row r="82" spans="1:7" ht="15.75" thickBot="1">
+    <row r="82" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1578,7 +1596,7 @@
       <c r="F82" s="7"/>
       <c r="G82" s="2"/>
     </row>
-    <row r="83" spans="1:7" ht="15.75" thickBot="1">
+    <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1590,7 +1608,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="2"/>
     </row>
-    <row r="84" spans="1:7" ht="15.75" thickBot="1">
+    <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="6"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1602,7 +1620,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="2"/>
     </row>
-    <row r="85" spans="1:7" ht="15.75" thickBot="1">
+    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="6"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1614,7 +1632,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="2"/>
     </row>
-    <row r="86" spans="1:7" ht="15.75" thickBot="1">
+    <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1626,7 +1644,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="2"/>
     </row>
-    <row r="87" spans="1:7" ht="15.75" thickBot="1">
+    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1638,7 +1656,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="2"/>
     </row>
-    <row r="88" spans="1:7" ht="15.75" thickBot="1">
+    <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1650,7 +1668,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="2"/>
     </row>
-    <row r="89" spans="1:7" ht="15.75" thickBot="1">
+    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1662,7 +1680,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="2"/>
     </row>
-    <row r="90" spans="1:7" ht="15.75" thickBot="1">
+    <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1674,7 +1692,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="2"/>
     </row>
-    <row r="91" spans="1:7" ht="15.75" thickBot="1">
+    <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1686,7 +1704,7 @@
       <c r="F91" s="7"/>
       <c r="G91" s="2"/>
     </row>
-    <row r="92" spans="1:7" ht="15.75" thickBot="1">
+    <row r="92" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1698,7 +1716,7 @@
       <c r="F92" s="7"/>
       <c r="G92" s="2"/>
     </row>
-    <row r="93" spans="1:7" ht="15.75" thickBot="1">
+    <row r="93" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1710,7 +1728,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="2"/>
     </row>
-    <row r="94" spans="1:7" ht="15.75" thickBot="1">
+    <row r="94" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1722,7 +1740,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="2"/>
     </row>
-    <row r="95" spans="1:7" ht="15.75" thickBot="1">
+    <row r="95" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1734,7 +1752,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="2"/>
     </row>
-    <row r="96" spans="1:7" ht="15.75" thickBot="1">
+    <row r="96" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1746,7 +1764,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="2"/>
     </row>
-    <row r="97" spans="1:7" ht="15.75" thickBot="1">
+    <row r="97" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1758,7 +1776,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="2"/>
     </row>
-    <row r="98" spans="1:7" ht="15.75" thickBot="1">
+    <row r="98" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1770,7 +1788,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="2"/>
     </row>
-    <row r="99" spans="1:7" ht="15.75" thickBot="1">
+    <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1782,7 +1800,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="2"/>
     </row>
-    <row r="100" spans="1:7" ht="15.75" thickBot="1">
+    <row r="100" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -1794,7 +1812,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="2"/>
     </row>
-    <row r="101" spans="1:7" ht="15.75" thickBot="1">
+    <row r="101" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -1806,7 +1824,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" ht="15.75" thickBot="1">
+    <row r="102" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -1818,7 +1836,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" ht="15.75" thickBot="1">
+    <row r="103" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -1830,7 +1848,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:7" ht="15.75" thickBot="1">
+    <row r="104" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -1842,7 +1860,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="2"/>
     </row>
-    <row r="105" spans="1:7" ht="15.75" thickBot="1">
+    <row r="105" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="6"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -1854,7 +1872,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="2"/>
     </row>
-    <row r="106" spans="1:7" ht="15.75" thickBot="1">
+    <row r="106" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -1866,7 +1884,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="2"/>
     </row>
-    <row r="107" spans="1:7" ht="15.75" thickBot="1">
+    <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="8"/>
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
@@ -1878,7 +1896,7 @@
       <c r="F107" s="10"/>
       <c r="G107" s="2"/>
     </row>
-    <row r="108" spans="1:7" ht="15.75" thickTop="1"/>
+    <row r="108" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>